<commit_message>
Add some unhappy case
</commit_message>
<xml_diff>
--- a/Excels/CreateTransferCheck02.xlsx
+++ b/Excels/CreateTransferCheck02.xlsx
@@ -87,28 +87,28 @@
     <t>Deposit</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>Con</t>
-  </si>
-  <si>
-    <t>10/01/1984</t>
-  </si>
-  <si>
-    <t>0 Moulton Court</t>
-  </si>
-  <si>
-    <t>Bryan</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t>cbarnardod@state.tx.us</t>
-  </si>
-  <si>
-    <t>e7enXPEjjhj</t>
+    <t>Aimil</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>11/04/1963</t>
+  </si>
+  <si>
+    <t>620 Mesta Way</t>
+  </si>
+  <si>
+    <t>Scottsdale</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>amcphatere@github.io</t>
+  </si>
+  <si>
+    <t>4khIDBFT5L</t>
   </si>
 </sst>
 </file>
@@ -518,10 +518,10 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -536,10 +536,10 @@
         <v>27</v>
       </c>
       <c r="G2">
-        <v>299893</v>
+        <v>863266</v>
       </c>
       <c r="H2">
-        <v>9798842872</v>
+        <v>4806825343</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>

</xml_diff>